<commit_message>
Refactoring reports (part 5)
</commit_message>
<xml_diff>
--- a/src/Phoenix.Services/Reports/Templates/PlcReport_en-US.xlsx
+++ b/src/Phoenix.Services/Reports/Templates/PlcReport_en-US.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maciej\Projekty\Phoenix\src\Phoenix.Services\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C021FE-1599-472B-B9C7-80891DC07C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0FD02B-4474-4C3C-AA42-FBE9D39C7304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -610,12 +610,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -754,11 +767,68 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -769,66 +839,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1162,13 +1183,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="68"/>
+      <c r="A1" s="50"/>
     </row>
     <row r="2" spans="1:1" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="68"/>
+      <c r="A2" s="50"/>
     </row>
     <row r="3" spans="1:1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68"/>
+      <c r="A3" s="50"/>
     </row>
     <row r="4" spans="1:1" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -3043,58 +3064,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70"/>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
+      <c r="A1" s="53"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
     </row>
     <row r="2" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="72"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
     </row>
     <row r="3" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="55" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55" t="s">
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55" t="s">
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
+      <c r="K3" s="56"/>
+      <c r="L3" s="56"/>
       <c r="M3" s="3" t="s">
         <v>9</v>
       </c>
@@ -3147,24 +3168,24 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="61" t="s">
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61" t="s">
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
       <c r="M5" s="14" t="s">
         <v>18</v>
       </c>
@@ -9073,7 +9094,7 @@
   <dimension ref="A1:ALE376"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9084,139 +9105,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69"/>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="70"/>
-      <c r="AG1" s="70"/>
+      <c r="A1" s="75"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="76"/>
+      <c r="AB1" s="76"/>
+      <c r="AC1" s="76"/>
+      <c r="AD1" s="76"/>
+      <c r="AE1" s="76"/>
+      <c r="AF1" s="76"/>
+      <c r="AG1" s="77"/>
     </row>
     <row r="2" spans="1:33" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="52" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="71" t="s">
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="71"/>
-      <c r="R2" s="71"/>
-      <c r="S2" s="71" t="s">
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="74"/>
+      <c r="S2" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="71"/>
-      <c r="U2" s="71"/>
-      <c r="V2" s="71"/>
-      <c r="W2" s="71"/>
-      <c r="X2" s="71"/>
-      <c r="Y2" s="71"/>
-      <c r="Z2" s="71"/>
-      <c r="AA2" s="71"/>
-      <c r="AB2" s="52" t="s">
+      <c r="T2" s="74"/>
+      <c r="U2" s="74"/>
+      <c r="V2" s="74"/>
+      <c r="W2" s="74"/>
+      <c r="X2" s="74"/>
+      <c r="Y2" s="74"/>
+      <c r="Z2" s="74"/>
+      <c r="AA2" s="74"/>
+      <c r="AB2" s="71" t="s">
         <v>23</v>
       </c>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
-      <c r="AF2" s="53"/>
-      <c r="AG2" s="54"/>
+      <c r="AC2" s="72"/>
+      <c r="AD2" s="72"/>
+      <c r="AE2" s="72"/>
+      <c r="AF2" s="72"/>
+      <c r="AG2" s="73"/>
     </row>
     <row r="3" spans="1:33" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50" t="s">
+      <c r="A3" s="70"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50" t="s">
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="56" t="s">
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="56"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="55" t="s">
+      <c r="K3" s="55"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="56"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="73" t="s">
+      <c r="N3" s="55"/>
+      <c r="O3" s="55"/>
+      <c r="P3" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
-      <c r="S3" s="56" t="s">
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="56"/>
-      <c r="U3" s="60"/>
-      <c r="V3" s="55" t="s">
+      <c r="T3" s="55"/>
+      <c r="U3" s="68"/>
+      <c r="V3" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="W3" s="56"/>
-      <c r="X3" s="56"/>
-      <c r="Y3" s="73" t="s">
+      <c r="W3" s="55"/>
+      <c r="X3" s="55"/>
+      <c r="Y3" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="Z3" s="73"/>
-      <c r="AA3" s="73"/>
-      <c r="AB3" s="60" t="s">
+      <c r="Z3" s="67"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="66"/>
-      <c r="AD3" s="74"/>
-      <c r="AE3" s="65" t="s">
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="69"/>
+      <c r="AE3" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="AF3" s="66"/>
-      <c r="AG3" s="67"/>
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="59"/>
     </row>
     <row r="4" spans="1:33" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -9320,55 +9341,55 @@
       </c>
     </row>
     <row r="5" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="51" t="s">
+      <c r="B5" s="60"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51" t="s">
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="57" t="s">
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="75" t="s">
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="64"/>
-      <c r="S5" s="57" t="s">
+      <c r="Q5" s="63"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="T5" s="58"/>
-      <c r="U5" s="58"/>
-      <c r="V5" s="58"/>
-      <c r="W5" s="58"/>
-      <c r="X5" s="59"/>
-      <c r="Y5" s="75" t="s">
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
+      <c r="X5" s="64"/>
+      <c r="Y5" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="Z5" s="58"/>
-      <c r="AA5" s="64"/>
-      <c r="AB5" s="51" t="s">
+      <c r="Z5" s="63"/>
+      <c r="AA5" s="66"/>
+      <c r="AB5" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="AC5" s="51"/>
-      <c r="AD5" s="51"/>
-      <c r="AE5" s="51"/>
-      <c r="AF5" s="51"/>
-      <c r="AG5" s="51"/>
+      <c r="AC5" s="61"/>
+      <c r="AD5" s="61"/>
+      <c r="AE5" s="61"/>
+      <c r="AF5" s="61"/>
+      <c r="AG5" s="61"/>
     </row>
     <row r="6" spans="1:33" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
@@ -22219,7 +22240,16 @@
     <row r="375" spans="1:33" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="376" spans="1:33" s="1" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="24">
+    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="J2:R2"/>
+    <mergeCell ref="S2:AA2"/>
+    <mergeCell ref="AB2:AG2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="A1:AG1"/>
     <mergeCell ref="AE3:AG3"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:F5"/>
@@ -22235,16 +22265,6 @@
     <mergeCell ref="V3:X3"/>
     <mergeCell ref="Y3:AA3"/>
     <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:AG1"/>
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="J2:R2"/>
-    <mergeCell ref="S2:AA2"/>
-    <mergeCell ref="AB2:AG2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="J3:L3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157505" right="0.39370078740157505" top="0.39370078740157505" bottom="0.39370078740157505" header="0.39370078740157505" footer="0.39370078740157505"/>

</xml_diff>

<commit_message>
Refactoring reports (part 6)
</commit_message>
<xml_diff>
--- a/src/Phoenix.Services/Reports/Templates/PlcReport_en-US.xlsx
+++ b/src/Phoenix.Services/Reports/Templates/PlcReport_en-US.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maciej\Projekty\Phoenix\src\Phoenix.Services\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0FD02B-4474-4C3C-AA42-FBE9D39C7304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E765E4-AC12-4072-A5C1-229F6CBE5D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="5" r:id="rId1"/>
@@ -788,6 +788,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -821,34 +839,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1171,7 +1171,7 @@
   </sheetPr>
   <dimension ref="A1:AJY376"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
@@ -9093,7 +9093,7 @@
   </sheetPr>
   <dimension ref="A1:ALE376"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:AG1"/>
     </sheetView>
   </sheetViews>
@@ -9140,104 +9140,104 @@
       <c r="AG1" s="77"/>
     </row>
     <row r="2" spans="1:33" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="71" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="74" t="s">
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="74"/>
-      <c r="N2" s="74"/>
-      <c r="O2" s="74"/>
-      <c r="P2" s="74"/>
-      <c r="Q2" s="74"/>
-      <c r="R2" s="74"/>
-      <c r="S2" s="74" t="s">
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="74"/>
-      <c r="U2" s="74"/>
-      <c r="V2" s="74"/>
-      <c r="W2" s="74"/>
-      <c r="X2" s="74"/>
-      <c r="Y2" s="74"/>
-      <c r="Z2" s="74"/>
-      <c r="AA2" s="74"/>
-      <c r="AB2" s="71" t="s">
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="61"/>
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="61"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AC2" s="72"/>
-      <c r="AD2" s="72"/>
-      <c r="AE2" s="72"/>
-      <c r="AF2" s="72"/>
-      <c r="AG2" s="73"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="59"/>
+      <c r="AF2" s="59"/>
+      <c r="AG2" s="60"/>
     </row>
     <row r="3" spans="1:33" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="70"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70" t="s">
+      <c r="A3" s="57"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70" t="s">
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
       <c r="J3" s="55" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="55"/>
-      <c r="L3" s="68"/>
+      <c r="L3" s="62"/>
       <c r="M3" s="56" t="s">
         <v>6</v>
       </c>
       <c r="N3" s="55"/>
       <c r="O3" s="55"/>
-      <c r="P3" s="67" t="s">
+      <c r="P3" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
+      <c r="Q3" s="73"/>
+      <c r="R3" s="73"/>
       <c r="S3" s="55" t="s">
         <v>3</v>
       </c>
       <c r="T3" s="55"/>
-      <c r="U3" s="68"/>
+      <c r="U3" s="62"/>
       <c r="V3" s="56" t="s">
         <v>6</v>
       </c>
       <c r="W3" s="55"/>
       <c r="X3" s="55"/>
-      <c r="Y3" s="67" t="s">
+      <c r="Y3" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="Z3" s="67"/>
-      <c r="AA3" s="67"/>
-      <c r="AB3" s="68" t="s">
+      <c r="Z3" s="73"/>
+      <c r="AA3" s="73"/>
+      <c r="AB3" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="69"/>
-      <c r="AE3" s="57" t="s">
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="74"/>
+      <c r="AE3" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="AF3" s="58"/>
-      <c r="AG3" s="59"/>
+      <c r="AF3" s="64"/>
+      <c r="AG3" s="65"/>
     </row>
     <row r="4" spans="1:33" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -9341,55 +9341,55 @@
       </c>
     </row>
     <row r="5" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61" t="s">
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61" t="s">
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="62" t="s">
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="64"/>
-      <c r="P5" s="65" t="s">
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="66"/>
-      <c r="S5" s="62" t="s">
+      <c r="Q5" s="69"/>
+      <c r="R5" s="72"/>
+      <c r="S5" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="T5" s="63"/>
-      <c r="U5" s="63"/>
-      <c r="V5" s="63"/>
-      <c r="W5" s="63"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="65" t="s">
+      <c r="T5" s="69"/>
+      <c r="U5" s="69"/>
+      <c r="V5" s="69"/>
+      <c r="W5" s="69"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="71" t="s">
         <v>15</v>
       </c>
-      <c r="Z5" s="63"/>
-      <c r="AA5" s="66"/>
-      <c r="AB5" s="61" t="s">
+      <c r="Z5" s="69"/>
+      <c r="AA5" s="72"/>
+      <c r="AB5" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="AC5" s="61"/>
-      <c r="AD5" s="61"/>
-      <c r="AE5" s="61"/>
-      <c r="AF5" s="61"/>
-      <c r="AG5" s="61"/>
+      <c r="AC5" s="67"/>
+      <c r="AD5" s="67"/>
+      <c r="AE5" s="67"/>
+      <c r="AF5" s="67"/>
+      <c r="AG5" s="67"/>
     </row>
     <row r="6" spans="1:33" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
@@ -22241,14 +22241,6 @@
     <row r="376" spans="1:33" s="1" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="J2:R2"/>
-    <mergeCell ref="S2:AA2"/>
-    <mergeCell ref="AB2:AG2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="J3:L3"/>
     <mergeCell ref="A1:AG1"/>
     <mergeCell ref="AE3:AG3"/>
     <mergeCell ref="A5:C5"/>
@@ -22265,6 +22257,14 @@
     <mergeCell ref="V3:X3"/>
     <mergeCell ref="Y3:AA3"/>
     <mergeCell ref="AB3:AD3"/>
+    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="J2:R2"/>
+    <mergeCell ref="S2:AA2"/>
+    <mergeCell ref="AB2:AG2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="J3:L3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157505" right="0.39370078740157505" top="0.39370078740157505" bottom="0.39370078740157505" header="0.39370078740157505" footer="0.39370078740157505"/>

</xml_diff>

<commit_message>
Refactoring reports (part 7)
</commit_message>
<xml_diff>
--- a/src/Phoenix.Services/Reports/Templates/PlcReport_en-US.xlsx
+++ b/src/Phoenix.Services/Reports/Templates/PlcReport_en-US.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maciej\Projekty\Phoenix\src\Phoenix.Services\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E765E4-AC12-4072-A5C1-229F6CBE5D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B92EC9-239C-497C-B1E3-84E72232735D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -768,7 +768,7 @@
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -777,7 +777,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -805,6 +805,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -841,15 +850,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9105,39 +9105,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="75"/>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="76"/>
-      <c r="U1" s="76"/>
-      <c r="V1" s="76"/>
-      <c r="W1" s="76"/>
-      <c r="X1" s="76"/>
-      <c r="Y1" s="76"/>
-      <c r="Z1" s="76"/>
-      <c r="AA1" s="76"/>
-      <c r="AB1" s="76"/>
-      <c r="AC1" s="76"/>
-      <c r="AD1" s="76"/>
-      <c r="AE1" s="76"/>
-      <c r="AF1" s="76"/>
-      <c r="AG1" s="77"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="64"/>
+      <c r="AA1" s="64"/>
+      <c r="AB1" s="64"/>
+      <c r="AC1" s="64"/>
+      <c r="AD1" s="64"/>
+      <c r="AE1" s="64"/>
+      <c r="AF1" s="64"/>
+      <c r="AG1" s="65"/>
     </row>
     <row r="2" spans="1:33" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
@@ -9208,11 +9208,11 @@
       </c>
       <c r="N3" s="55"/>
       <c r="O3" s="55"/>
-      <c r="P3" s="73" t="s">
+      <c r="P3" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="73"/>
-      <c r="R3" s="73"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76"/>
       <c r="S3" s="55" t="s">
         <v>3</v>
       </c>
@@ -9223,21 +9223,21 @@
       </c>
       <c r="W3" s="55"/>
       <c r="X3" s="55"/>
-      <c r="Y3" s="73" t="s">
+      <c r="Y3" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="Z3" s="73"/>
-      <c r="AA3" s="73"/>
+      <c r="Z3" s="76"/>
+      <c r="AA3" s="76"/>
       <c r="AB3" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="74"/>
-      <c r="AE3" s="63" t="s">
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="77"/>
+      <c r="AE3" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="AF3" s="64"/>
-      <c r="AG3" s="65"/>
+      <c r="AF3" s="67"/>
+      <c r="AG3" s="68"/>
     </row>
     <row r="4" spans="1:33" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -9341,55 +9341,55 @@
       </c>
     </row>
     <row r="5" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="66" t="s">
+      <c r="A5" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="67" t="s">
+      <c r="B5" s="69"/>
+      <c r="C5" s="69"/>
+      <c r="D5" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67" t="s">
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="68" t="s">
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="71" t="s">
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="72"/>
+      <c r="O5" s="73"/>
+      <c r="P5" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="72"/>
-      <c r="S5" s="68" t="s">
+      <c r="Q5" s="72"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="T5" s="69"/>
-      <c r="U5" s="69"/>
-      <c r="V5" s="69"/>
-      <c r="W5" s="69"/>
-      <c r="X5" s="70"/>
-      <c r="Y5" s="71" t="s">
+      <c r="T5" s="72"/>
+      <c r="U5" s="72"/>
+      <c r="V5" s="72"/>
+      <c r="W5" s="72"/>
+      <c r="X5" s="73"/>
+      <c r="Y5" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="Z5" s="69"/>
-      <c r="AA5" s="72"/>
-      <c r="AB5" s="67" t="s">
+      <c r="Z5" s="72"/>
+      <c r="AA5" s="75"/>
+      <c r="AB5" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="AC5" s="67"/>
-      <c r="AD5" s="67"/>
-      <c r="AE5" s="67"/>
-      <c r="AF5" s="67"/>
-      <c r="AG5" s="67"/>
+      <c r="AC5" s="70"/>
+      <c r="AD5" s="70"/>
+      <c r="AE5" s="70"/>
+      <c r="AF5" s="70"/>
+      <c r="AG5" s="70"/>
     </row>
     <row r="6" spans="1:33" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>

</xml_diff>

<commit_message>
Refactoring reports (part 8)
</commit_message>
<xml_diff>
--- a/src/Phoenix.Services/Reports/Templates/PlcReport_en-US.xlsx
+++ b/src/Phoenix.Services/Reports/Templates/PlcReport_en-US.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Maciej\Projekty\Phoenix\src\Phoenix.Services\Reports\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B92EC9-239C-497C-B1E3-84E72232735D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D96672-74D5-41BA-8F2D-D73B53DBB352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -788,24 +788,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -848,7 +830,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9105,139 +9105,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
-      <c r="S1" s="64"/>
-      <c r="T1" s="64"/>
-      <c r="U1" s="64"/>
-      <c r="V1" s="64"/>
-      <c r="W1" s="64"/>
-      <c r="X1" s="64"/>
-      <c r="Y1" s="64"/>
-      <c r="Z1" s="64"/>
-      <c r="AA1" s="64"/>
-      <c r="AB1" s="64"/>
-      <c r="AC1" s="64"/>
-      <c r="AD1" s="64"/>
-      <c r="AE1" s="64"/>
-      <c r="AF1" s="64"/>
-      <c r="AG1" s="65"/>
+      <c r="A1" s="57"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="58"/>
+      <c r="U1" s="58"/>
+      <c r="V1" s="58"/>
+      <c r="W1" s="58"/>
+      <c r="X1" s="58"/>
+      <c r="Y1" s="58"/>
+      <c r="Z1" s="58"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="59"/>
     </row>
     <row r="2" spans="1:33" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="58" t="s">
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61" t="s">
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="61"/>
-      <c r="O2" s="61"/>
-      <c r="P2" s="61"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="61"/>
-      <c r="S2" s="61" t="s">
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61"/>
-      <c r="V2" s="61"/>
-      <c r="W2" s="61"/>
-      <c r="X2" s="61"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="61"/>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="58" t="s">
+      <c r="T2" s="77"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="77"/>
+      <c r="X2" s="77"/>
+      <c r="Y2" s="77"/>
+      <c r="Z2" s="77"/>
+      <c r="AA2" s="77"/>
+      <c r="AB2" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="AC2" s="59"/>
-      <c r="AD2" s="59"/>
-      <c r="AE2" s="59"/>
-      <c r="AF2" s="59"/>
-      <c r="AG2" s="60"/>
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="75"/>
+      <c r="AE2" s="75"/>
+      <c r="AF2" s="75"/>
+      <c r="AG2" s="76"/>
     </row>
     <row r="3" spans="1:33" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57" t="s">
+      <c r="A3" s="73"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57" t="s">
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
       <c r="J3" s="55" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="55"/>
-      <c r="L3" s="62"/>
+      <c r="L3" s="71"/>
       <c r="M3" s="56" t="s">
         <v>6</v>
       </c>
       <c r="N3" s="55"/>
       <c r="O3" s="55"/>
-      <c r="P3" s="76" t="s">
+      <c r="P3" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="76"/>
-      <c r="R3" s="76"/>
+      <c r="Q3" s="70"/>
+      <c r="R3" s="70"/>
       <c r="S3" s="55" t="s">
         <v>3</v>
       </c>
       <c r="T3" s="55"/>
-      <c r="U3" s="62"/>
+      <c r="U3" s="71"/>
       <c r="V3" s="56" t="s">
         <v>6</v>
       </c>
       <c r="W3" s="55"/>
       <c r="X3" s="55"/>
-      <c r="Y3" s="76" t="s">
+      <c r="Y3" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="Z3" s="76"/>
-      <c r="AA3" s="76"/>
-      <c r="AB3" s="62" t="s">
+      <c r="Z3" s="70"/>
+      <c r="AA3" s="70"/>
+      <c r="AB3" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="67"/>
-      <c r="AD3" s="77"/>
-      <c r="AE3" s="66" t="s">
+      <c r="AC3" s="61"/>
+      <c r="AD3" s="72"/>
+      <c r="AE3" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="AF3" s="67"/>
-      <c r="AG3" s="68"/>
+      <c r="AF3" s="61"/>
+      <c r="AG3" s="62"/>
     </row>
     <row r="4" spans="1:33" ht="78" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -9341,55 +9341,55 @@
       </c>
     </row>
     <row r="5" spans="1:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="69" t="s">
+      <c r="A5" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="70" t="s">
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70" t="s">
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="71" t="s">
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="72"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="74" t="s">
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="72"/>
-      <c r="R5" s="75"/>
-      <c r="S5" s="71" t="s">
+      <c r="Q5" s="66"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="T5" s="72"/>
-      <c r="U5" s="72"/>
-      <c r="V5" s="72"/>
-      <c r="W5" s="72"/>
-      <c r="X5" s="73"/>
-      <c r="Y5" s="74" t="s">
+      <c r="T5" s="66"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="66"/>
+      <c r="W5" s="66"/>
+      <c r="X5" s="67"/>
+      <c r="Y5" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="Z5" s="72"/>
-      <c r="AA5" s="75"/>
-      <c r="AB5" s="70" t="s">
+      <c r="Z5" s="66"/>
+      <c r="AA5" s="69"/>
+      <c r="AB5" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="AC5" s="70"/>
-      <c r="AD5" s="70"/>
-      <c r="AE5" s="70"/>
-      <c r="AF5" s="70"/>
-      <c r="AG5" s="70"/>
+      <c r="AC5" s="64"/>
+      <c r="AD5" s="64"/>
+      <c r="AE5" s="64"/>
+      <c r="AF5" s="64"/>
+      <c r="AG5" s="64"/>
     </row>
     <row r="6" spans="1:33" ht="28.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
@@ -22241,6 +22241,14 @@
     <row r="376" spans="1:33" s="1" customFormat="1" ht="90.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="J2:R2"/>
+    <mergeCell ref="S2:AA2"/>
+    <mergeCell ref="AB2:AG2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="J3:L3"/>
     <mergeCell ref="A1:AG1"/>
     <mergeCell ref="AE3:AG3"/>
     <mergeCell ref="A5:C5"/>
@@ -22257,14 +22265,6 @@
     <mergeCell ref="V3:X3"/>
     <mergeCell ref="Y3:AA3"/>
     <mergeCell ref="AB3:AD3"/>
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="D2:I2"/>
-    <mergeCell ref="J2:R2"/>
-    <mergeCell ref="S2:AA2"/>
-    <mergeCell ref="AB2:AG2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="J3:L3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.39370078740157505" right="0.39370078740157505" top="0.39370078740157505" bottom="0.39370078740157505" header="0.39370078740157505" footer="0.39370078740157505"/>

</xml_diff>